<commit_message>
Add new class device, debug, polish files, improve library
Add class device: grid-forming inverter.
Debug: InstallSimplexPS.
</commit_message>
<xml_diff>
--- a/Examples/paper_port coupling/PortCoupling_SingleVSIInfiniteBus.xlsx
+++ b/Examples/paper_port coupling/PortCoupling_SingleVSIInfiniteBus.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Power-System-Analysis-Toolbox\Examples\data for paper_port coupling\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Power-System-Analysis-Toolbox\Examples\paper_port coupling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FBAE4A4-391A-42B7-8006-CB32C442E2C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E06DE43E-9EAA-4DCB-B4BC-B04FAAC65DFF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PowerFlow" sheetId="1" r:id="rId1"/>
@@ -793,8 +793,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -1471,7 +1471,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EFCB373-2341-40B6-A375-7BA50357479A}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>

</xml_diff>